<commit_message>
Update data files - Bot run at 2026-02-12 04:49:57 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,67 +434,67 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>User_ID</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Requests per Minute</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Requests per Day</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Tokens per Minute</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Tokens per Day</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Current_Ct_Day</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Current_Pct_Ct</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Current_Ct_Tokens</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Current_Pct_Tokens</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Last_Reset</t>
         </is>
@@ -522,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0007638888888888889</v>
+        <v>0.0008333333333333334</v>
       </c>
       <c r="K2" t="n">
-        <v>2730</v>
+        <v>3213</v>
       </c>
       <c r="L2" t="n">
-        <v>0.00546</v>
+        <v>0.006426</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 07:56:11 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0009027777777777777</v>
+        <v>0.0009722222222222222</v>
       </c>
       <c r="K2" t="n">
-        <v>3690</v>
+        <v>4157</v>
       </c>
       <c r="L2" t="n">
-        <v>0.00738</v>
+        <v>0.008314</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 10:38:45 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -891,16 +891,16 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K9" t="n">
-        <v>68</v>
+        <v>307</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0002266666666666667</v>
+        <v>0.001023333333333333</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
@@ -993,16 +993,16 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K11" t="n">
-        <v>51</v>
+        <v>286</v>
       </c>
       <c r="L11" t="n">
-        <v>0.000255</v>
+        <v>0.00143</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
@@ -1044,16 +1044,16 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K12" t="n">
-        <v>51</v>
+        <v>519</v>
       </c>
       <c r="L12" t="n">
-        <v>0.000255</v>
+        <v>0.002595</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 11:43:54 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" t="n">
-        <v>0.001041666666666667</v>
+        <v>0.001111111111111111</v>
       </c>
       <c r="K2" t="n">
-        <v>4400</v>
+        <v>4868</v>
       </c>
       <c r="L2" t="n">
-        <v>0.008800000000000001</v>
+        <v>0.009736</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -585,16 +585,16 @@
         <v>100000</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K3" t="n">
-        <v>77</v>
+        <v>712</v>
       </c>
       <c r="L3" t="n">
-        <v>0.00077</v>
+        <v>0.00712</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 13:20:01 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" t="n">
-        <v>0.001111111111111111</v>
+        <v>0.001180555555555556</v>
       </c>
       <c r="K2" t="n">
-        <v>4868</v>
+        <v>5381</v>
       </c>
       <c r="L2" t="n">
-        <v>0.009736</v>
+        <v>0.010762</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 18:31:34 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -585,16 +585,16 @@
         <v>100000</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>469</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>0.00469</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 19:50:49 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -636,16 +636,16 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>494</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>0.0009879999999999999</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 21:39:07 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -891,16 +891,16 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>486</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>0.00162</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 04:57:55 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
-        <v>6.944444444444444e-05</v>
+        <v>0.0001388888888888889</v>
       </c>
       <c r="K2" t="n">
-        <v>472</v>
+        <v>937</v>
       </c>
       <c r="L2" t="n">
-        <v>0.000944</v>
+        <v>0.001874</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -1146,16 +1146,16 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>483</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>0.000966</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 08:51:46 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0002083333333333333</v>
+        <v>0.0002777777777777778</v>
       </c>
       <c r="K2" t="n">
-        <v>1409</v>
+        <v>1922</v>
       </c>
       <c r="L2" t="n">
-        <v>0.002818</v>
+        <v>0.003844</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 21:06:20 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,20 +534,20 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0002777777777777778</v>
+        <v>6.944444444444444e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>1922</v>
+        <v>476</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003844</v>
+        <v>0.000952</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -591,14 +591,14 @@
         <v>0.001</v>
       </c>
       <c r="K3" t="n">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="L3" t="n">
-        <v>0.00469</v>
+        <v>0.00472</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -636,20 +636,20 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>494</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0009879999999999999</v>
+        <v>0</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -687,20 +687,20 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>713</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.001426</v>
+        <v>0</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -802,7 +802,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -891,20 +891,20 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>486</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.00162</v>
+        <v>0</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -942,20 +942,20 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>532</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0.001773333333333333</v>
+        <v>0</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -993,20 +993,20 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>562</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.00281</v>
+        <v>0</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -1044,20 +1044,20 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>475</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.002375</v>
+        <v>0</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>
@@ -1146,20 +1146,20 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>483</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0.000966</v>
+        <v>0</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-18T21:06:08.465605</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 21:58:41 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -636,16 +636,16 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>471</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>0.000942</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -687,16 +687,16 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>472</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>0.000944</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 22:45:00 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -891,16 +891,16 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>481</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>0.001603333333333333</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-18 23:35:38 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -942,16 +942,16 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>469</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.001563333333333333</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -993,16 +993,16 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>469</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.002345</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 02:37:07 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -1044,16 +1044,16 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>695</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>0.003475</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 04:57:10 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -1146,16 +1146,16 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>0.000946</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 07:33:29 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
-        <v>6.944444444444444e-05</v>
+        <v>0.0001388888888888889</v>
       </c>
       <c r="K2" t="n">
-        <v>476</v>
+        <v>953</v>
       </c>
       <c r="L2" t="n">
-        <v>0.000952</v>
+        <v>0.001906</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 09:54:48 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0001388888888888889</v>
+        <v>0.0002083333333333333</v>
       </c>
       <c r="K2" t="n">
-        <v>953</v>
+        <v>1426</v>
       </c>
       <c r="L2" t="n">
-        <v>0.001906</v>
+        <v>0.002852</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 10:51:47 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0002083333333333333</v>
+        <v>0.0003472222222222222</v>
       </c>
       <c r="K2" t="n">
-        <v>1426</v>
+        <v>2487</v>
       </c>
       <c r="L2" t="n">
-        <v>0.002852</v>
+        <v>0.004974</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 11:42:25 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0003472222222222222</v>
+        <v>0.0004166666666666667</v>
       </c>
       <c r="K2" t="n">
-        <v>2487</v>
+        <v>2969</v>
       </c>
       <c r="L2" t="n">
-        <v>0.004974</v>
+        <v>0.005938</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 13:17:33 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0004166666666666667</v>
+        <v>0.0005555555555555556</v>
       </c>
       <c r="K2" t="n">
-        <v>2969</v>
+        <v>3909</v>
       </c>
       <c r="L2" t="n">
-        <v>0.005938</v>
+        <v>0.007818</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 14:31:27 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0005555555555555556</v>
+        <v>0.000625</v>
       </c>
       <c r="K2" t="n">
-        <v>3909</v>
+        <v>4425</v>
       </c>
       <c r="L2" t="n">
-        <v>0.007818</v>
+        <v>0.00885</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 17:00:35 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J2" t="n">
-        <v>0.000625</v>
+        <v>0.0008333333333333334</v>
       </c>
       <c r="K2" t="n">
-        <v>4425</v>
+        <v>5835</v>
       </c>
       <c r="L2" t="n">
-        <v>0.00885</v>
+        <v>0.01167</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 17:57:22 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0008333333333333334</v>
+        <v>0.001041666666666667</v>
       </c>
       <c r="K2" t="n">
-        <v>5835</v>
+        <v>7268</v>
       </c>
       <c r="L2" t="n">
-        <v>0.01167</v>
+        <v>0.014536</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 19:02:56 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -636,16 +636,16 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K4" t="n">
-        <v>471</v>
+        <v>1016</v>
       </c>
       <c r="L4" t="n">
-        <v>0.000942</v>
+        <v>0.002032</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 19:58:56 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -687,16 +687,16 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K5" t="n">
-        <v>472</v>
+        <v>948</v>
       </c>
       <c r="L5" t="n">
-        <v>0.000944</v>
+        <v>0.001896</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 20:43:47 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -942,16 +942,16 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K10" t="n">
-        <v>469</v>
+        <v>945</v>
       </c>
       <c r="L10" t="n">
-        <v>0.001563333333333333</v>
+        <v>0.00315</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -1146,16 +1146,16 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K14" t="n">
-        <v>473</v>
+        <v>939</v>
       </c>
       <c r="L14" t="n">
-        <v>0.000946</v>
+        <v>0.001878</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-19 22:38:15 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,20 +534,20 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.001041666666666667</v>
+        <v>6.944444444444444e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>7268</v>
+        <v>501</v>
       </c>
       <c r="L2" t="n">
-        <v>0.014536</v>
+        <v>0.001002</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -591,14 +591,14 @@
         <v>0.001</v>
       </c>
       <c r="K3" t="n">
-        <v>472</v>
+        <v>505</v>
       </c>
       <c r="L3" t="n">
-        <v>0.00472</v>
+        <v>0.00505</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -636,20 +636,20 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>1016</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.002032</v>
+        <v>0</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -687,20 +687,20 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>948</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.001896</v>
+        <v>0</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -802,7 +802,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -891,20 +891,20 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>481</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.001603333333333333</v>
+        <v>0</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -942,20 +942,20 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>945</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0.00315</v>
+        <v>0</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -993,20 +993,20 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>469</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.002345</v>
+        <v>0</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -1044,20 +1044,20 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>695</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.003475</v>
+        <v>0</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>
@@ -1146,20 +1146,20 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>939</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0.001878</v>
+        <v>0</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2026-02-18T21:06:08.465605</t>
+          <t>2026-02-19T22:38:03.628800</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 05:57:52 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -636,16 +636,16 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>635</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>0.00127</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 07:08:27 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -687,16 +687,16 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>470</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>0.00094</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 08:03:37 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -891,16 +891,16 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>0.001576666666666667</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 11:06:25 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -942,16 +942,16 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>477</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.00159</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 11:55:20 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -993,16 +993,16 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>471</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.002355</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 14:11:48 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -1044,16 +1044,16 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>470</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>0.00235</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 17:08:43 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -1146,16 +1146,16 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>465</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>0.0009300000000000001</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 19:21:11 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
-        <v>6.944444444444444e-05</v>
+        <v>0.0001388888888888889</v>
       </c>
       <c r="K2" t="n">
-        <v>501</v>
+        <v>966</v>
       </c>
       <c r="L2" t="n">
-        <v>0.001002</v>
+        <v>0.001932</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 19:54:03 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0001388888888888889</v>
+        <v>0.0002083333333333333</v>
       </c>
       <c r="K2" t="n">
-        <v>966</v>
+        <v>1439</v>
       </c>
       <c r="L2" t="n">
-        <v>0.001932</v>
+        <v>0.002878</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 20:38:52 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0002083333333333333</v>
+        <v>0.0002777777777777778</v>
       </c>
       <c r="K2" t="n">
-        <v>1439</v>
+        <v>1912</v>
       </c>
       <c r="L2" t="n">
-        <v>0.002878</v>
+        <v>0.003824</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 21:30:48 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0002777777777777778</v>
+        <v>0.0004861111111111111</v>
       </c>
       <c r="K2" t="n">
-        <v>1912</v>
+        <v>3331</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003824</v>
+        <v>0.006662</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-20 23:33:55 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,20 +534,20 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0004861111111111111</v>
+        <v>6.944444444444444e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>3331</v>
+        <v>469</v>
       </c>
       <c r="L2" t="n">
-        <v>0.006662</v>
+        <v>0.000938</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -591,14 +591,14 @@
         <v>0.001</v>
       </c>
       <c r="K3" t="n">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="L3" t="n">
-        <v>0.00505</v>
+        <v>0.00495</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -636,20 +636,20 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>635</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.00127</v>
+        <v>0</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -687,20 +687,20 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>470</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.00094</v>
+        <v>0</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -802,7 +802,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -891,20 +891,20 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>473</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.001576666666666667</v>
+        <v>0</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -942,20 +942,20 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>477</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0.00159</v>
+        <v>0</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -993,20 +993,20 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>471</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.002355</v>
+        <v>0</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -1044,20 +1044,20 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>470</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.00235</v>
+        <v>0</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>
@@ -1146,20 +1146,20 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>465</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0009300000000000001</v>
+        <v>0</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2026-02-19T22:38:03.628800</t>
+          <t>2026-02-20T23:33:43.608782</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 02:25:59 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -636,16 +636,16 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>684</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>0.001368</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 04:18:03 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -687,16 +687,16 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>537</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>0.001074</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 06:05:00 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -891,16 +891,16 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>481</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>0.001603333333333333</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 07:08:36 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -942,16 +942,16 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>465</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.00155</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 07:53:14 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -993,16 +993,16 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>477</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.002385</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 08:37:44 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -1044,16 +1044,16 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>475</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>0.002375</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 11:27:03 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
-        <v>6.944444444444444e-05</v>
+        <v>0.0001388888888888889</v>
       </c>
       <c r="K2" t="n">
-        <v>469</v>
+        <v>937</v>
       </c>
       <c r="L2" t="n">
-        <v>0.000938</v>
+        <v>0.001874</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -1146,16 +1146,16 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>527</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>0.001054</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 12:58:32 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0001388888888888889</v>
+        <v>0.0002777777777777778</v>
       </c>
       <c r="K2" t="n">
-        <v>937</v>
+        <v>1888</v>
       </c>
       <c r="L2" t="n">
-        <v>0.001874</v>
+        <v>0.003776</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 13:49:43 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0002777777777777778</v>
+        <v>0.0004166666666666667</v>
       </c>
       <c r="K2" t="n">
-        <v>1888</v>
+        <v>3002</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003776</v>
+        <v>0.006004</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 14:31:19 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0004166666666666667</v>
+        <v>0.0004861111111111111</v>
       </c>
       <c r="K2" t="n">
-        <v>3002</v>
+        <v>3474</v>
       </c>
       <c r="L2" t="n">
-        <v>0.006004</v>
+        <v>0.006948</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 17:29:57 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0004861111111111111</v>
+        <v>0.0005555555555555556</v>
       </c>
       <c r="K2" t="n">
-        <v>3474</v>
+        <v>3939</v>
       </c>
       <c r="L2" t="n">
-        <v>0.006948</v>
+        <v>0.007878</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 19:49:15 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0005555555555555556</v>
+        <v>0.0006944444444444445</v>
       </c>
       <c r="K2" t="n">
-        <v>3939</v>
+        <v>4974</v>
       </c>
       <c r="L2" t="n">
-        <v>0.007878</v>
+        <v>0.009948</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 21:28:48 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0006944444444444445</v>
+        <v>0.0007638888888888889</v>
       </c>
       <c r="K2" t="n">
-        <v>4974</v>
+        <v>5440</v>
       </c>
       <c r="L2" t="n">
-        <v>0.009948</v>
+        <v>0.01088</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 21:50:31 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0007638888888888889</v>
+        <v>0.0009027777777777777</v>
       </c>
       <c r="K2" t="n">
-        <v>5440</v>
+        <v>6396</v>
       </c>
       <c r="L2" t="n">
-        <v>0.01088</v>
+        <v>0.012792</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 22:30:13 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0009027777777777777</v>
+        <v>0.001041666666666667</v>
       </c>
       <c r="K2" t="n">
-        <v>6396</v>
+        <v>7364</v>
       </c>
       <c r="L2" t="n">
-        <v>0.012792</v>
+        <v>0.014728</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 23:29:35 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -1146,16 +1146,16 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K14" t="n">
-        <v>527</v>
+        <v>1007</v>
       </c>
       <c r="L14" t="n">
-        <v>0.001054</v>
+        <v>0.002014</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-21 23:51:03 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,20 +534,20 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.001041666666666667</v>
+        <v>6.944444444444444e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>7364</v>
+        <v>480</v>
       </c>
       <c r="L2" t="n">
-        <v>0.014728</v>
+        <v>0.00096</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -585,20 +585,20 @@
         <v>100000</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>495</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.00495</v>
+        <v>0</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -636,20 +636,20 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>684</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.001368</v>
+        <v>0</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -687,20 +687,20 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>537</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.001074</v>
+        <v>0</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -802,7 +802,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -891,20 +891,20 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>481</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.001603333333333333</v>
+        <v>0</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -942,20 +942,20 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>465</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0.00155</v>
+        <v>0</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -993,20 +993,20 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>477</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.002385</v>
+        <v>0</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -1044,20 +1044,20 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>475</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.002375</v>
+        <v>0</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>
@@ -1146,20 +1146,20 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>1007</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0.002014</v>
+        <v>0</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2026-02-20T23:33:43.608782</t>
+          <t>2026-02-21T23:50:55.774358</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 02:37:33 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -585,16 +585,16 @@
         <v>100000</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>684</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>0.00684</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 04:53:14 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -636,16 +636,16 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>475</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>0.00095</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 05:55:19 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -687,16 +687,16 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>491</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>0.000982</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 09:36:43 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -891,16 +891,16 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>504</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>0.00168</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 13:50:38 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -942,16 +942,16 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>483</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.00161</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 14:31:28 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -993,16 +993,16 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>508</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.00254</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
@@ -1044,16 +1044,16 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>508</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>0.00254</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 17:29:53 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -1146,16 +1146,16 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>466</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>0.000932</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 17:54:47 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>6.944444444444444e-05</v>
+        <v>0.0002777777777777778</v>
       </c>
       <c r="K2" t="n">
-        <v>480</v>
+        <v>1891</v>
       </c>
       <c r="L2" t="n">
-        <v>0.00096</v>
+        <v>0.003782</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 18:42:41 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0002777777777777778</v>
+        <v>0.0004166666666666667</v>
       </c>
       <c r="K2" t="n">
-        <v>1891</v>
+        <v>2835</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003782</v>
+        <v>0.00567</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 19:30:25 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0004166666666666667</v>
+        <v>0.000625</v>
       </c>
       <c r="K2" t="n">
-        <v>2835</v>
+        <v>4265</v>
       </c>
       <c r="L2" t="n">
-        <v>0.00567</v>
+        <v>0.008529999999999999</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 19:50:07 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J2" t="n">
-        <v>0.000625</v>
+        <v>0.0008333333333333334</v>
       </c>
       <c r="K2" t="n">
-        <v>4265</v>
+        <v>5691</v>
       </c>
       <c r="L2" t="n">
-        <v>0.008529999999999999</v>
+        <v>0.011382</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-22 20:33:47 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0008333333333333334</v>
+        <v>0.001041666666666667</v>
       </c>
       <c r="K2" t="n">
-        <v>5691</v>
+        <v>7122</v>
       </c>
       <c r="L2" t="n">
-        <v>0.011382</v>
+        <v>0.014244</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>